<commit_message>
(2.0.0.132): AVSOfficeDocxFile2 (1.0.0.55): XlsxSerializerCom setFontDir для PPTXFile::IAVSOfficeDrawingConverter(ошибки при открытии chart), открытие TxPr для legend, default шрифт для header chart.
git-svn-id: svn://192.168.3.15/activex/AVS/Sources/TeamlabOffice/trunk/OfficeWeb@47637 954022d7-b5bf-4e40-9824-e11837661b57
</commit_message>
<xml_diff>
--- a/Excel/offlinedocs/test-chart-font-setting.xlsx
+++ b/Excel/offlinedocs/test-chart-font-setting.xlsx
@@ -184,11 +184,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="142392320"/>
-        <c:axId val="142402688"/>
+        <c:axId val="142388224"/>
+        <c:axId val="142398592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="142392320"/>
+        <c:axId val="142388224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -224,7 +224,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142402688"/>
+        <c:crossAx val="142398592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -232,7 +232,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142402688"/>
+        <c:axId val="142398592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -278,7 +278,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142392320"/>
+        <c:crossAx val="142388224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -495,11 +495,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="142640256"/>
-        <c:axId val="142642176"/>
+        <c:axId val="142648448"/>
+        <c:axId val="142650368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="142640256"/>
+        <c:axId val="142648448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -541,7 +541,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142642176"/>
+        <c:crossAx val="142650368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -549,7 +549,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142642176"/>
+        <c:axId val="142650368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -595,7 +595,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142640256"/>
+        <c:crossAx val="142648448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -629,6 +629,156 @@
       <a:noFill/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>asd</a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$2:$D$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$3:$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="146090624"/>
+        <c:axId val="146272640"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="146090624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="146272640"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="146272640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="146090624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -696,6 +846,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Диаграмма 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -994,7 +1174,7 @@
   <dimension ref="B2:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>